<commit_message>
updated other excel file just for consistency
</commit_message>
<xml_diff>
--- a/NTA Hospitalization Rates.xlsx
+++ b/NTA Hospitalization Rates.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rocky\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rocky\Desktop\Comp-Epi-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74DEAC4E-5CA6-478B-B181-EAF1EB65DFCF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A38CE2E-138E-43E3-B000-71EB6970BF40}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AC33AD24-C5F0-4647-8D15-2B73697B8E29}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AC33AD24-C5F0-4647-8D15-2B73697B8E29}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1594,7 +1594,7 @@
   <dimension ref="A1:N188"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B115" sqref="B115"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1704,8 +1704,8 @@
         <v>7325.2659999999996</v>
       </c>
       <c r="N3">
-        <f>((K3*0.081)+(L3*0.052)+(M3*0.022))/C3</f>
-        <v>5.0473999999999998E-2</v>
+        <f>((K3*0.00445172)+(L3*0.00452715)+(M3*0.00458679))/C3</f>
+        <v>4.5270547600000004E-3</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
@@ -1746,8 +1746,8 @@
         <v>5641.1970000000001</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N4:N65" si="3">((K4*0.081)+(L4*0.052)+(M4*0.022))/C4</f>
-        <v>5.2787000000000001E-2</v>
+        <f t="shared" ref="N4:N67" si="3">((K4*0.00445172)+(L4*0.00452715)+(M4*0.00458679))/C4</f>
+        <v>4.5262159199999999E-3</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -1789,7 +1789,7 @@
       </c>
       <c r="N5">
         <f t="shared" si="3"/>
-        <v>4.3262000000000002E-2</v>
+        <v>4.5385394900000001E-3</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -1831,7 +1831,7 @@
       </c>
       <c r="N6">
         <f t="shared" si="3"/>
-        <v>5.5099000000000002E-2</v>
+        <v>4.5163491299999997E-3</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -1873,7 +1873,7 @@
       </c>
       <c r="N7">
         <f t="shared" si="3"/>
-        <v>5.1938999999999999E-2</v>
+        <v>4.5235201100000009E-3</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -1915,7 +1915,7 @@
       </c>
       <c r="N8">
         <f t="shared" si="3"/>
-        <v>5.3036E-2</v>
+        <v>4.5168687500000007E-3</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -1957,7 +1957,7 @@
       </c>
       <c r="N9">
         <f t="shared" si="3"/>
-        <v>5.3649999999999996E-2</v>
+        <v>4.5201364200000002E-3</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -1999,7 +1999,7 @@
       </c>
       <c r="N10">
         <f t="shared" si="3"/>
-        <v>5.2507999999999999E-2</v>
+        <v>4.5181317499999995E-3</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -2041,7 +2041,7 @@
       </c>
       <c r="N11">
         <f t="shared" si="3"/>
-        <v>5.3992999999999992E-2</v>
+        <v>4.5239250599999996E-3</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
@@ -2083,7 +2083,7 @@
       </c>
       <c r="N12">
         <f t="shared" si="3"/>
-        <v>5.3745000000000008E-2</v>
+        <v>4.5200364499999998E-3</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
@@ -2125,7 +2125,7 @@
       </c>
       <c r="N13">
         <f t="shared" si="3"/>
-        <v>5.6279999999999997E-2</v>
+        <v>4.5099574500000001E-3</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
@@ -2167,7 +2167,7 @@
       </c>
       <c r="N14">
         <f t="shared" si="3"/>
-        <v>5.4249000000000012E-2</v>
+        <v>4.5194611700000008E-3</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
@@ -2209,7 +2209,7 @@
       </c>
       <c r="N15">
         <f t="shared" si="3"/>
-        <v>5.7111999999999982E-2</v>
+        <v>4.5124006199999999E-3</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
@@ -2251,7 +2251,7 @@
       </c>
       <c r="N16">
         <f t="shared" si="3"/>
-        <v>5.5728999999999994E-2</v>
+        <v>4.5108572799999998E-3</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="N17">
         <f t="shared" si="3"/>
-        <v>5.4924000000000008E-2</v>
+        <v>4.5226253500000001E-3</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
@@ -2335,7 +2335,7 @@
       </c>
       <c r="N18">
         <f t="shared" si="3"/>
-        <v>5.4749000000000006E-2</v>
+        <v>4.5230621400000007E-3</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
@@ -2377,7 +2377,7 @@
       </c>
       <c r="N19">
         <f t="shared" si="3"/>
-        <v>5.4439999999999988E-2</v>
+        <v>4.5187436799999994E-3</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
@@ -2419,7 +2419,7 @@
       </c>
       <c r="N20">
         <f t="shared" si="3"/>
-        <v>5.6905999999999998E-2</v>
+        <v>4.5171206699999994E-3</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
@@ -2461,7 +2461,7 @@
       </c>
       <c r="N21">
         <f t="shared" si="3"/>
-        <v>5.5724000000000003E-2</v>
+        <v>4.5155510800000001E-3</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
@@ -2503,7 +2503,7 @@
       </c>
       <c r="N22">
         <f t="shared" si="3"/>
-        <v>5.5257000000000001E-2</v>
+        <v>4.5114044999999998E-3</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
@@ -2545,7 +2545,7 @@
       </c>
       <c r="N23">
         <f t="shared" si="3"/>
-        <v>5.2968000000000001E-2</v>
+        <v>4.52163446E-3</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
@@ -2587,7 +2587,7 @@
       </c>
       <c r="N24">
         <f t="shared" si="3"/>
-        <v>5.4577000000000001E-2</v>
+        <v>4.5177068699999998E-3</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
@@ -2629,7 +2629,7 @@
       </c>
       <c r="N25">
         <f t="shared" si="3"/>
-        <v>5.6287999999999984E-2</v>
+        <v>4.5180292499999988E-3</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
@@ -2671,7 +2671,7 @@
       </c>
       <c r="N26">
         <f t="shared" si="3"/>
-        <v>5.5525999999999999E-2</v>
+        <v>4.5113852899999994E-3</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.35">
@@ -2713,7 +2713,7 @@
       </c>
       <c r="N27">
         <f t="shared" si="3"/>
-        <v>5.4821000000000002E-2</v>
+        <v>4.5268384100000001E-3</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
@@ -2755,7 +2755,7 @@
       </c>
       <c r="N28">
         <f t="shared" si="3"/>
-        <v>5.4322000000000002E-2</v>
+        <v>4.5232532299999996E-3</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.35">
@@ -2797,7 +2797,7 @@
       </c>
       <c r="N29">
         <f t="shared" si="3"/>
-        <v>5.5173999999999994E-2</v>
+        <v>4.5122272899999994E-3</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.35">
@@ -2839,7 +2839,7 @@
       </c>
       <c r="N30">
         <f t="shared" si="3"/>
-        <v>5.5916999999999994E-2</v>
+        <v>4.5196379199999998E-3</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.35">
@@ -2881,7 +2881,7 @@
       </c>
       <c r="N31">
         <f t="shared" si="3"/>
-        <v>5.3091000000000006E-2</v>
+        <v>4.5225099499999998E-3</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.35">
@@ -2923,7 +2923,7 @@
       </c>
       <c r="N32">
         <f t="shared" si="3"/>
-        <v>5.3597999999999993E-2</v>
+        <v>4.5161426100000001E-3</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.35">
@@ -2965,7 +2965,7 @@
       </c>
       <c r="N33">
         <f t="shared" si="3"/>
-        <v>5.4460000000000001E-2</v>
+        <v>4.5190594799999996E-3</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.35">
@@ -3007,7 +3007,7 @@
       </c>
       <c r="N34">
         <f t="shared" si="3"/>
-        <v>6.3321000000000002E-2</v>
+        <v>4.4963059700000004E-3</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.35">
@@ -3049,7 +3049,7 @@
       </c>
       <c r="N35">
         <f t="shared" si="3"/>
-        <v>5.5051000000000003E-2</v>
+        <v>4.5087124099999999E-3</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.35">
@@ -3091,7 +3091,7 @@
       </c>
       <c r="N36">
         <f t="shared" si="3"/>
-        <v>5.8397999999999999E-2</v>
+        <v>4.5044668499999996E-3</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.35">
@@ -3133,7 +3133,7 @@
       </c>
       <c r="N37">
         <f t="shared" si="3"/>
-        <v>5.2183000000000007E-2</v>
+        <v>4.5156940099999997E-3</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.35">
@@ -3175,7 +3175,7 @@
       </c>
       <c r="N38">
         <f t="shared" si="3"/>
-        <v>5.7315999999999999E-2</v>
+        <v>4.5076489899999999E-3</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.35">
@@ -3217,7 +3217,7 @@
       </c>
       <c r="N39">
         <f t="shared" si="3"/>
-        <v>5.5741999999999993E-2</v>
+        <v>4.5110625500000001E-3</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.35">
@@ -3259,7 +3259,7 @@
       </c>
       <c r="N40">
         <f t="shared" si="3"/>
-        <v>5.6611999999999996E-2</v>
+        <v>4.5178118100000003E-3</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.35">
@@ -3301,7 +3301,7 @@
       </c>
       <c r="N41">
         <f t="shared" si="3"/>
-        <v>5.811199999999999E-2</v>
+        <v>4.5095237200000002E-3</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.35">
@@ -3343,7 +3343,7 @@
       </c>
       <c r="N42">
         <f t="shared" si="3"/>
-        <v>5.7560000000000007E-2</v>
+        <v>4.5109411000000006E-3</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.35">
@@ -3385,7 +3385,7 @@
       </c>
       <c r="N43">
         <f t="shared" si="3"/>
-        <v>5.7952999999999991E-2</v>
+        <v>4.5149858999999999E-3</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.35">
@@ -3427,7 +3427,7 @@
       </c>
       <c r="N44">
         <f t="shared" si="3"/>
-        <v>5.9114E-2</v>
+        <v>4.5119844899999999E-3</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.35">
@@ -3469,7 +3469,7 @@
       </c>
       <c r="N45">
         <f t="shared" si="3"/>
-        <v>6.0663999999999989E-2</v>
+        <v>4.5028858799999998E-3</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.35">
@@ -3511,7 +3511,7 @@
       </c>
       <c r="N46">
         <f t="shared" si="3"/>
-        <v>5.1992000000000003E-2</v>
+        <v>4.5248903199999989E-3</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.35">
@@ -3553,7 +3553,7 @@
       </c>
       <c r="N47">
         <f t="shared" si="3"/>
-        <v>5.3599999999999995E-2</v>
+        <v>4.5156408499999997E-3</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.35">
@@ -3595,7 +3595,7 @@
       </c>
       <c r="N48">
         <f t="shared" si="3"/>
-        <v>5.0538E-2</v>
+        <v>4.5264653E-3</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.35">
@@ -3637,7 +3637,7 @@
       </c>
       <c r="N49">
         <f t="shared" si="3"/>
-        <v>5.5485E-2</v>
+        <v>4.5112712399999998E-3</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.35">
@@ -3679,7 +3679,7 @@
       </c>
       <c r="N50">
         <f t="shared" si="3"/>
-        <v>5.4407000000000004E-2</v>
+        <v>4.5229953599999996E-3</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.35">
@@ -3721,7 +3721,7 @@
       </c>
       <c r="N51">
         <f t="shared" si="3"/>
-        <v>5.9229000000000004E-2</v>
+        <v>4.5068942300000008E-3</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.35">
@@ -3763,7 +3763,7 @@
       </c>
       <c r="N52">
         <f t="shared" si="3"/>
-        <v>5.5929E-2</v>
+        <v>4.5055091499999998E-3</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.35">
@@ -3805,7 +3805,7 @@
       </c>
       <c r="N53">
         <f t="shared" si="3"/>
-        <v>5.7194000000000002E-2</v>
+        <v>4.5168681300000006E-3</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.35">
@@ -3847,7 +3847,7 @@
       </c>
       <c r="N54">
         <f t="shared" si="3"/>
-        <v>5.7831999999999995E-2</v>
+        <v>4.5014237599999996E-3</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.35">
@@ -3889,7 +3889,7 @@
       </c>
       <c r="N55">
         <f t="shared" si="3"/>
-        <v>5.5481999999999997E-2</v>
+        <v>4.5159966200000005E-3</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.35">
@@ -3931,7 +3931,7 @@
       </c>
       <c r="N56">
         <f t="shared" si="3"/>
-        <v>5.6991000000000007E-2</v>
+        <v>4.5078506399999999E-3</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.35">
@@ -3973,7 +3973,7 @@
       </c>
       <c r="N57">
         <f t="shared" si="3"/>
-        <v>5.4743E-2</v>
+        <v>4.51288856E-3</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.35">
@@ -4015,7 +4015,7 @@
       </c>
       <c r="N58">
         <f t="shared" si="3"/>
-        <v>5.1391000000000006E-2</v>
+        <v>4.5297733999999992E-3</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.35">
@@ -4057,7 +4057,7 @@
       </c>
       <c r="N59">
         <f t="shared" si="3"/>
-        <v>5.0541000000000003E-2</v>
+        <v>4.5270460099999998E-3</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.35">
@@ -4099,7 +4099,7 @@
       </c>
       <c r="N60">
         <f t="shared" si="3"/>
-        <v>5.6538000000000005E-2</v>
+        <v>4.5086978699999999E-3</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.35">
@@ -4141,7 +4141,7 @@
       </c>
       <c r="N61">
         <f t="shared" si="3"/>
-        <v>5.832699999999999E-2</v>
+        <v>4.5044124400000001E-3</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.35">
@@ -4183,7 +4183,7 @@
       </c>
       <c r="N62">
         <f t="shared" si="3"/>
-        <v>5.1074000000000001E-2</v>
+        <v>4.5348741200000008E-3</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.35">
@@ -4225,7 +4225,7 @@
       </c>
       <c r="N63">
         <f t="shared" si="3"/>
-        <v>5.9060000000000008E-2</v>
+        <v>4.5074257599999994E-3</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.35">
@@ -4267,7 +4267,7 @@
       </c>
       <c r="N64">
         <f t="shared" si="3"/>
-        <v>5.7871999999999993E-2</v>
+        <v>4.5195463400000005E-3</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.35">
@@ -4309,7 +4309,7 @@
       </c>
       <c r="N65">
         <f t="shared" si="3"/>
-        <v>5.5476999999999992E-2</v>
+        <v>4.5254631699999989E-3</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.35">
@@ -4350,8 +4350,8 @@
         <v>6161.0640000000003</v>
       </c>
       <c r="N66">
-        <f t="shared" ref="N66:N129" si="7">((K66*0.081)+(L66*0.052)+(M66*0.022))/C66</f>
-        <v>5.1977999999999996E-2</v>
+        <f t="shared" si="3"/>
+        <v>4.5236025800000001E-3</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.35">
@@ -4392,8 +4392,8 @@
         <v>3129.1520000000005</v>
       </c>
       <c r="N67">
-        <f t="shared" si="7"/>
-        <v>5.5804999999999993E-2</v>
+        <f t="shared" si="3"/>
+        <v>4.5200027999999998E-3</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.35">
@@ -4434,8 +4434,8 @@
         <v>5889.5519999999997</v>
       </c>
       <c r="N68">
-        <f t="shared" si="7"/>
-        <v>5.2991999999999997E-2</v>
+        <f t="shared" ref="N68:N131" si="7">((K68*0.00445172)+(L68*0.00452715)+(M68*0.00458679))/C68</f>
+        <v>4.5167073299999996E-3</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.35">
@@ -4477,7 +4477,7 @@
       </c>
       <c r="N69">
         <f t="shared" si="7"/>
-        <v>5.8152000000000002E-2</v>
+        <v>4.5096219799999997E-3</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.35">
@@ -4519,7 +4519,7 @@
       </c>
       <c r="N70">
         <f t="shared" si="7"/>
-        <v>5.8522999999999999E-2</v>
+        <v>4.5085466499999996E-3</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.35">
@@ -4561,7 +4561,7 @@
       </c>
       <c r="N71">
         <f t="shared" si="7"/>
-        <v>5.8202999999999991E-2</v>
+        <v>4.4955756799999989E-3</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.35">
@@ -4603,7 +4603,7 @@
       </c>
       <c r="N72">
         <f t="shared" si="7"/>
-        <v>5.7528999999999983E-2</v>
+        <v>4.5067455399999991E-3</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.35">
@@ -4645,7 +4645,7 @@
       </c>
       <c r="N73">
         <f t="shared" si="7"/>
-        <v>5.7002999999999998E-2</v>
+        <v>4.5122795299999997E-3</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.35">
@@ -4687,7 +4687,7 @@
       </c>
       <c r="N74">
         <f t="shared" si="7"/>
-        <v>5.858E-2</v>
+        <v>4.5131527499999999E-3</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.35">
@@ -4729,7 +4729,7 @@
       </c>
       <c r="N75">
         <f t="shared" si="7"/>
-        <v>5.9159000000000003E-2</v>
+        <v>4.5026161999999993E-3</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.35">
@@ -4771,7 +4771,7 @@
       </c>
       <c r="N76">
         <f t="shared" si="7"/>
-        <v>5.8138000000000002E-2</v>
+        <v>4.50993426E-3</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.35">
@@ -4813,7 +4813,7 @@
       </c>
       <c r="N77">
         <f t="shared" si="7"/>
-        <v>5.729999999999999E-2</v>
+        <v>4.5116357599999995E-3</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.35">
@@ -4855,7 +4855,7 @@
       </c>
       <c r="N78">
         <f t="shared" si="7"/>
-        <v>5.6297E-2</v>
+        <v>4.5139319500000002E-3</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.35">
@@ -4897,7 +4897,7 @@
       </c>
       <c r="N79">
         <f t="shared" si="7"/>
-        <v>5.5050000000000009E-2</v>
+        <v>4.51717544E-3</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.35">
@@ -4939,7 +4939,7 @@
       </c>
       <c r="N80">
         <f t="shared" si="7"/>
-        <v>5.424699999999999E-2</v>
+        <v>4.514123499999999E-3</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.35">
@@ -4981,7 +4981,7 @@
       </c>
       <c r="N81">
         <f t="shared" si="7"/>
-        <v>5.3894999999999992E-2</v>
+        <v>4.5287504099999999E-3</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.35">
@@ -5023,7 +5023,7 @@
       </c>
       <c r="N82">
         <f t="shared" si="7"/>
-        <v>5.6757999999999996E-2</v>
+        <v>4.51745045E-3</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.35">
@@ -5065,7 +5065,7 @@
       </c>
       <c r="N83">
         <f t="shared" si="7"/>
-        <v>5.6522999999999997E-2</v>
+        <v>4.5089943599999991E-3</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.35">
@@ -5107,7 +5107,7 @@
       </c>
       <c r="N84">
         <f t="shared" si="7"/>
-        <v>5.4685000000000004E-2</v>
+        <v>4.5178121699999997E-3</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.35">
@@ -5149,7 +5149,7 @@
       </c>
       <c r="N85">
         <f t="shared" si="7"/>
-        <v>5.8211999999999993E-2</v>
+        <v>4.514275449999999E-3</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.35">
@@ -5191,7 +5191,7 @@
       </c>
       <c r="N86">
         <f t="shared" si="7"/>
-        <v>5.8606000000000005E-2</v>
+        <v>4.4992450400000005E-3</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.35">
@@ -5233,7 +5233,7 @@
       </c>
       <c r="N87">
         <f t="shared" si="7"/>
-        <v>5.5001000000000001E-2</v>
+        <v>4.5174684100000003E-3</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.35">
@@ -5275,7 +5275,7 @@
       </c>
       <c r="N88">
         <f t="shared" si="7"/>
-        <v>5.5204999999999997E-2</v>
+        <v>4.5169561900000009E-3</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.35">
@@ -5317,7 +5317,7 @@
       </c>
       <c r="N89">
         <f t="shared" si="7"/>
-        <v>5.4534999999999993E-2</v>
+        <v>4.5186437099999999E-3</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.35">
@@ -5359,7 +5359,7 @@
       </c>
       <c r="N90">
         <f t="shared" si="7"/>
-        <v>5.4088999999999998E-2</v>
+        <v>4.5196014700000006E-3</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.35">
@@ -5401,7 +5401,7 @@
       </c>
       <c r="N91">
         <f t="shared" si="7"/>
-        <v>5.2031999999999995E-2</v>
+        <v>4.5249885799999992E-3</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.35">
@@ -5443,7 +5443,7 @@
       </c>
       <c r="N92">
         <f t="shared" si="7"/>
-        <v>5.5272999999999996E-2</v>
+        <v>4.5169632299999997E-3</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.35">
@@ -5485,7 +5485,7 @@
       </c>
       <c r="N93">
         <f t="shared" si="7"/>
-        <v>5.1450000000000003E-2</v>
+        <v>4.5253989199999997E-3</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.35">
@@ -5527,7 +5527,7 @@
       </c>
       <c r="N94">
         <f t="shared" si="7"/>
-        <v>5.1943999999999997E-2</v>
+        <v>4.5299718300000008E-3</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.35">
@@ -5569,7 +5569,7 @@
       </c>
       <c r="N95">
         <f t="shared" si="7"/>
-        <v>5.0616000000000001E-2</v>
+        <v>4.5181514199999998E-3</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.35">
@@ -5611,7 +5611,7 @@
       </c>
       <c r="N96">
         <f t="shared" si="7"/>
-        <v>5.0370999999999999E-2</v>
+        <v>4.5339345200000004E-3</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.35">
@@ -5653,7 +5653,7 @@
       </c>
       <c r="N97">
         <f t="shared" si="7"/>
-        <v>4.9715999999999996E-2</v>
+        <v>4.5305527999999996E-3</v>
       </c>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.35">
@@ -5695,7 +5695,7 @@
       </c>
       <c r="N98">
         <f t="shared" si="7"/>
-        <v>4.7629999999999999E-2</v>
+        <v>4.5344153200000004E-3</v>
       </c>
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.35">
@@ -5737,7 +5737,7 @@
       </c>
       <c r="N99">
         <f t="shared" si="7"/>
-        <v>5.0583000000000003E-2</v>
+        <v>4.5330152800000011E-3</v>
       </c>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.35">
@@ -5779,7 +5779,7 @@
       </c>
       <c r="N100">
         <f t="shared" si="7"/>
-        <v>5.0297999999999995E-2</v>
+        <v>4.5200636199999996E-3</v>
       </c>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.35">
@@ -5821,7 +5821,7 @@
       </c>
       <c r="N101">
         <f t="shared" si="7"/>
-        <v>5.0893000000000001E-2</v>
+        <v>4.5283373699999997E-3</v>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.35">
@@ -5863,7 +5863,7 @@
       </c>
       <c r="N102">
         <f t="shared" si="7"/>
-        <v>5.0383999999999998E-2</v>
+        <v>4.5288337000000001E-3</v>
       </c>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.35">
@@ -5905,7 +5905,7 @@
       </c>
       <c r="N103">
         <f t="shared" si="7"/>
-        <v>5.2697000000000001E-2</v>
+        <v>4.5232221099999999E-3</v>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.35">
@@ -5947,7 +5947,7 @@
       </c>
       <c r="N104">
         <f t="shared" si="7"/>
-        <v>5.4133999999999988E-2</v>
+        <v>4.5250847699999999E-3</v>
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.35">
@@ -5989,7 +5989,7 @@
       </c>
       <c r="N105">
         <f t="shared" si="7"/>
-        <v>5.1329E-2</v>
+        <v>4.5213822799999998E-3</v>
       </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.35">
@@ -6031,7 +6031,7 @@
       </c>
       <c r="N106">
         <f t="shared" si="7"/>
-        <v>5.1595999999999996E-2</v>
+        <v>4.5250375599999995E-3</v>
       </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.35">
@@ -6073,7 +6073,7 @@
       </c>
       <c r="N107">
         <f t="shared" si="7"/>
-        <v>5.0846999999999996E-2</v>
+        <v>4.5270776899999999E-3</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.35">
@@ -6115,7 +6115,7 @@
       </c>
       <c r="N108">
         <f t="shared" si="7"/>
-        <v>5.0646999999999998E-2</v>
+        <v>4.5276530699999993E-3</v>
       </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.35">
@@ -6157,7 +6157,7 @@
       </c>
       <c r="N109">
         <f t="shared" si="7"/>
-        <v>5.3552999999999989E-2</v>
+        <v>4.5207381500000001E-3</v>
       </c>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.35">
@@ -6199,7 +6199,7 @@
       </c>
       <c r="N110">
         <f t="shared" si="7"/>
-        <v>5.5661999999999989E-2</v>
+        <v>4.5108660300000004E-3</v>
       </c>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.35">
@@ -6241,7 +6241,7 @@
       </c>
       <c r="N111">
         <f t="shared" si="7"/>
-        <v>5.2948999999999996E-2</v>
+        <v>4.5176283799999994E-3</v>
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.35">
@@ -6283,7 +6283,7 @@
       </c>
       <c r="N112">
         <f t="shared" si="7"/>
-        <v>5.3415999999999991E-2</v>
+        <v>4.5212416199999989E-3</v>
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.35">
@@ -6325,7 +6325,7 @@
       </c>
       <c r="N113">
         <f t="shared" si="7"/>
-        <v>4.9545999999999993E-2</v>
+        <v>4.5241624300000009E-3</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.35">
@@ -6367,7 +6367,7 @@
       </c>
       <c r="N114">
         <f t="shared" si="7"/>
-        <v>4.9410000000000003E-2</v>
+        <v>4.5352938700000001E-3</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.35">
@@ -6409,7 +6409,7 @@
       </c>
       <c r="N115">
         <f t="shared" si="7"/>
-        <v>5.8172999999999996E-2</v>
+        <v>4.5094202299999992E-3</v>
       </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.35">
@@ -6451,7 +6451,7 @@
       </c>
       <c r="N116">
         <f t="shared" si="7"/>
-        <v>5.4436999999999992E-2</v>
+        <v>4.5181629699999996E-3</v>
       </c>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.35">
@@ -6493,7 +6493,7 @@
       </c>
       <c r="N117">
         <f t="shared" si="7"/>
-        <v>5.5809999999999998E-2</v>
+        <v>4.5153090000000003E-3</v>
       </c>
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.35">
@@ -6535,7 +6535,7 @@
       </c>
       <c r="N118">
         <f t="shared" si="7"/>
-        <v>5.6230000000000002E-2</v>
+        <v>4.5097012900000002E-3</v>
       </c>
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.35">
@@ -6577,7 +6577,7 @@
       </c>
       <c r="N119">
         <f t="shared" si="7"/>
-        <v>5.2517999999999995E-2</v>
+        <v>4.5273018099999994E-3</v>
       </c>
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.35">
@@ -6619,7 +6619,7 @@
       </c>
       <c r="N120">
         <f t="shared" si="7"/>
-        <v>5.352800000000002E-2</v>
+        <v>4.51610399E-3</v>
       </c>
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.35">
@@ -6661,7 +6661,7 @@
       </c>
       <c r="N121">
         <f t="shared" si="7"/>
-        <v>5.4690999999999997E-2</v>
+        <v>4.5131341599999996E-3</v>
       </c>
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.35">
@@ -6703,7 +6703,7 @@
       </c>
       <c r="N122">
         <f t="shared" si="7"/>
-        <v>5.3385000000000002E-2</v>
+        <v>4.5202187900000006E-3</v>
       </c>
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.35">
@@ -6745,7 +6745,7 @@
       </c>
       <c r="N123">
         <f t="shared" si="7"/>
-        <v>5.6880000000000007E-2</v>
+        <v>4.5076979700000002E-3</v>
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.35">
@@ -6787,7 +6787,7 @@
       </c>
       <c r="N124">
         <f t="shared" si="7"/>
-        <v>5.6111999999999995E-2</v>
+        <v>4.5046653399999992E-3</v>
       </c>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.35">
@@ -6829,7 +6829,7 @@
       </c>
       <c r="N125">
         <f t="shared" si="7"/>
-        <v>5.1711000000000007E-2</v>
+        <v>4.5199473000000013E-3</v>
       </c>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.35">
@@ -6871,7 +6871,7 @@
       </c>
       <c r="N126">
         <f t="shared" si="7"/>
-        <v>5.0835999999999999E-2</v>
+        <v>4.5221312499999994E-3</v>
       </c>
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.35">
@@ -6913,7 +6913,7 @@
       </c>
       <c r="N127">
         <f t="shared" si="7"/>
-        <v>5.4085999999999988E-2</v>
+        <v>4.5100086000000005E-3</v>
       </c>
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.35">
@@ -6955,7 +6955,7 @@
       </c>
       <c r="N128">
         <f t="shared" si="7"/>
-        <v>5.5943E-2</v>
+        <v>4.5105029600000009E-3</v>
       </c>
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.35">
@@ -6997,7 +6997,7 @@
       </c>
       <c r="N129">
         <f t="shared" si="7"/>
-        <v>5.1680999999999998E-2</v>
+        <v>4.5337918500000006E-3</v>
       </c>
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.35">
@@ -7038,8 +7038,8 @@
         <v>11652.038</v>
       </c>
       <c r="N130">
-        <f t="shared" ref="N130:N188" si="11">((K130*0.081)+(L130*0.052)+(M130*0.022))/C130</f>
-        <v>5.1311999999999997E-2</v>
+        <f t="shared" si="7"/>
+        <v>4.5258865999999991E-3</v>
       </c>
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.35">
@@ -7080,8 +7080,8 @@
         <v>3365.1420000000003</v>
       </c>
       <c r="N131">
-        <f t="shared" si="11"/>
-        <v>5.4302000000000003E-2</v>
+        <f t="shared" si="7"/>
+        <v>4.5186980200000006E-3</v>
       </c>
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.35">
@@ -7122,8 +7122,8 @@
         <v>5943.6</v>
       </c>
       <c r="N132">
-        <f t="shared" si="11"/>
-        <v>5.6065999999999998E-2</v>
+        <f t="shared" ref="N132:N188" si="11">((K132*0.00445172)+(L132*0.00452715)+(M132*0.00458679))/C132</f>
+        <v>4.5193239299999993E-3</v>
       </c>
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.35">
@@ -7165,7 +7165,7 @@
       </c>
       <c r="N133">
         <f t="shared" si="11"/>
-        <v>5.7604999999999996E-2</v>
+        <v>4.5068788999999996E-3</v>
       </c>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.35">
@@ -7207,7 +7207,7 @@
       </c>
       <c r="N134">
         <f t="shared" si="11"/>
-        <v>5.5174000000000001E-2</v>
+        <v>4.5170000400000009E-3</v>
       </c>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.35">
@@ -7249,7 +7249,7 @@
       </c>
       <c r="N135">
         <f t="shared" si="11"/>
-        <v>5.3617999999999999E-2</v>
+        <v>4.5159250699999993E-3</v>
       </c>
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.35">
@@ -7291,7 +7291,7 @@
       </c>
       <c r="N136">
         <f t="shared" si="11"/>
-        <v>5.4467000000000008E-2</v>
+        <v>4.52340942E-3</v>
       </c>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.35">
@@ -7333,7 +7333,7 @@
       </c>
       <c r="N137">
         <f t="shared" si="11"/>
-        <v>5.3379000000000003E-2</v>
+        <v>4.5164179800000004E-3</v>
       </c>
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.35">
@@ -7375,7 +7375,7 @@
       </c>
       <c r="N138">
         <f t="shared" si="11"/>
-        <v>5.3799999999999994E-2</v>
+        <v>4.5161321500000002E-3</v>
       </c>
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.35">
@@ -7417,7 +7417,7 @@
       </c>
       <c r="N139">
         <f t="shared" si="11"/>
-        <v>5.0969999999999994E-2</v>
+        <v>4.5215804099999991E-3</v>
       </c>
     </row>
     <row r="140" spans="1:14" x14ac:dyDescent="0.35">
@@ -7459,7 +7459,7 @@
       </c>
       <c r="N140">
         <f t="shared" si="11"/>
-        <v>5.4075999999999985E-2</v>
+        <v>4.5193962000000002E-3</v>
       </c>
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.35">
@@ -7501,7 +7501,7 @@
       </c>
       <c r="N141">
         <f t="shared" si="11"/>
-        <v>5.3624000000000005E-2</v>
+        <v>4.5160198099999998E-3</v>
       </c>
     </row>
     <row r="142" spans="1:14" x14ac:dyDescent="0.35">
@@ -7543,7 +7543,7 @@
       </c>
       <c r="N142">
         <f t="shared" si="11"/>
-        <v>5.4770000000000006E-2</v>
+        <v>4.51278155E-3</v>
       </c>
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.35">
@@ -7585,7 +7585,7 @@
       </c>
       <c r="N143">
         <f t="shared" si="11"/>
-        <v>5.4391000000000002E-2</v>
+        <v>4.5185033100000006E-3</v>
       </c>
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.35">
@@ -7627,7 +7627,7 @@
       </c>
       <c r="N144">
         <f t="shared" si="11"/>
-        <v>5.3677999999999997E-2</v>
+        <v>4.5200451999999995E-3</v>
       </c>
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.35">
@@ -7669,7 +7669,7 @@
       </c>
       <c r="N145">
         <f t="shared" si="11"/>
-        <v>5.2926000000000001E-2</v>
+        <v>4.5262773699999998E-3</v>
       </c>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.35">
@@ -7711,7 +7711,7 @@
       </c>
       <c r="N146">
         <f t="shared" si="11"/>
-        <v>5.3927000000000003E-2</v>
+        <v>4.5197101899999998E-3</v>
       </c>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.35">
@@ -7753,7 +7753,7 @@
       </c>
       <c r="N147">
         <f t="shared" si="11"/>
-        <v>4.8925000000000003E-2</v>
+        <v>4.5213175699999998E-3</v>
       </c>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.35">
@@ -7795,7 +7795,7 @@
       </c>
       <c r="N148">
         <f t="shared" si="11"/>
-        <v>5.2195999999999992E-2</v>
+        <v>4.5233114199999995E-3</v>
       </c>
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.35">
@@ -7837,7 +7837,7 @@
       </c>
       <c r="N149">
         <f t="shared" si="11"/>
-        <v>5.2638999999999991E-2</v>
+        <v>4.5270790399999988E-3</v>
       </c>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.35">
@@ -7879,7 +7879,7 @@
       </c>
       <c r="N150">
         <f t="shared" si="11"/>
-        <v>4.8641999999999998E-2</v>
+        <v>4.5311945600000009E-3</v>
       </c>
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.35">
@@ -7921,7 +7921,7 @@
       </c>
       <c r="N151">
         <f t="shared" si="11"/>
-        <v>5.2527999999999998E-2</v>
+        <v>4.5226869600000002E-3</v>
       </c>
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.35">
@@ -7963,7 +7963,7 @@
       </c>
       <c r="N152">
         <f t="shared" si="11"/>
-        <v>5.1684000000000008E-2</v>
+        <v>4.524293720000001E-3</v>
       </c>
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.35">
@@ -8005,7 +8005,7 @@
       </c>
       <c r="N153">
         <f t="shared" si="11"/>
-        <v>5.3661999999999994E-2</v>
+        <v>4.5160864899999997E-3</v>
       </c>
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.35">
@@ -8047,7 +8047,7 @@
       </c>
       <c r="N154">
         <f t="shared" si="11"/>
-        <v>5.1766E-2</v>
+        <v>4.52929457E-3</v>
       </c>
     </row>
     <row r="155" spans="1:14" x14ac:dyDescent="0.35">
@@ -8089,7 +8089,7 @@
       </c>
       <c r="N155">
         <f t="shared" si="11"/>
-        <v>5.2602000000000003E-2</v>
+        <v>4.5227887400000003E-3</v>
       </c>
     </row>
     <row r="156" spans="1:14" x14ac:dyDescent="0.35">
@@ -8131,7 +8131,7 @@
       </c>
       <c r="N156">
         <f t="shared" si="11"/>
-        <v>5.6501000000000003E-2</v>
+        <v>4.5091803200000002E-3</v>
       </c>
     </row>
     <row r="157" spans="1:14" x14ac:dyDescent="0.35">
@@ -8173,7 +8173,7 @@
       </c>
       <c r="N157">
         <f t="shared" si="11"/>
-        <v>5.6085999999999997E-2</v>
+        <v>4.5148669799999997E-3</v>
       </c>
     </row>
     <row r="158" spans="1:14" x14ac:dyDescent="0.35">
@@ -8215,7 +8215,7 @@
       </c>
       <c r="N158">
         <f t="shared" si="11"/>
-        <v>5.5148999999999997E-2</v>
+        <v>4.512365879999999E-3</v>
       </c>
     </row>
     <row r="159" spans="1:14" x14ac:dyDescent="0.35">
@@ -8257,7 +8257,7 @@
       </c>
       <c r="N159">
         <f t="shared" si="11"/>
-        <v>5.5451999999999994E-2</v>
+        <v>4.5160562599999999E-3</v>
       </c>
     </row>
     <row r="160" spans="1:14" x14ac:dyDescent="0.35">
@@ -8299,7 +8299,7 @@
       </c>
       <c r="N160">
         <f t="shared" si="11"/>
-        <v>5.0886999999999995E-2</v>
+        <v>4.5213365199999987E-3</v>
       </c>
     </row>
     <row r="161" spans="1:14" x14ac:dyDescent="0.35">
@@ -8341,7 +8341,7 @@
       </c>
       <c r="N161">
         <f t="shared" si="11"/>
-        <v>5.3331999999999997E-2</v>
+        <v>4.5305274400000003E-3</v>
       </c>
     </row>
     <row r="162" spans="1:14" x14ac:dyDescent="0.35">
@@ -8383,7 +8383,7 @@
       </c>
       <c r="N162">
         <f t="shared" si="11"/>
-        <v>5.5569999999999987E-2</v>
+        <v>4.5157861199999995E-3</v>
       </c>
     </row>
     <row r="163" spans="1:14" x14ac:dyDescent="0.35">
@@ -8425,7 +8425,7 @@
       </c>
       <c r="N163">
         <f t="shared" si="11"/>
-        <v>5.3691000000000003E-2</v>
+        <v>4.5250232199999995E-3</v>
       </c>
     </row>
     <row r="164" spans="1:14" x14ac:dyDescent="0.35">
@@ -8467,7 +8467,7 @@
       </c>
       <c r="N164">
         <f t="shared" si="11"/>
-        <v>5.4132999999999987E-2</v>
+        <v>4.5149901400000003E-3</v>
       </c>
     </row>
     <row r="165" spans="1:14" x14ac:dyDescent="0.35">
@@ -8509,7 +8509,7 @@
       </c>
       <c r="N165">
         <f t="shared" si="11"/>
-        <v>5.3495000000000001E-2</v>
+        <v>4.5203556700000001E-3</v>
       </c>
     </row>
     <row r="166" spans="1:14" x14ac:dyDescent="0.35">
@@ -8551,7 +8551,7 @@
       </c>
       <c r="N166">
         <f t="shared" si="11"/>
-        <v>5.5715999999999988E-2</v>
+        <v>4.5111853499999995E-3</v>
       </c>
     </row>
     <row r="167" spans="1:14" x14ac:dyDescent="0.35">
@@ -8593,7 +8593,7 @@
       </c>
       <c r="N167">
         <f t="shared" si="11"/>
-        <v>5.1885999999999995E-2</v>
+        <v>4.5343620999999997E-3</v>
       </c>
     </row>
     <row r="168" spans="1:14" x14ac:dyDescent="0.35">
@@ -8635,7 +8635,7 @@
       </c>
       <c r="N168">
         <f t="shared" si="11"/>
-        <v>5.3911000000000001E-2</v>
+        <v>4.5109787300000002E-3</v>
       </c>
     </row>
     <row r="169" spans="1:14" x14ac:dyDescent="0.35">
@@ -8677,7 +8677,7 @@
       </c>
       <c r="N169">
         <f t="shared" si="11"/>
-        <v>5.2658999999999997E-2</v>
+        <v>4.5231554300000001E-3</v>
       </c>
     </row>
     <row r="170" spans="1:14" x14ac:dyDescent="0.35">
@@ -8719,7 +8719,7 @@
       </c>
       <c r="N170">
         <f t="shared" si="11"/>
-        <v>5.5892999999999991E-2</v>
+        <v>4.5150195499999999E-3</v>
       </c>
     </row>
     <row r="171" spans="1:14" x14ac:dyDescent="0.35">
@@ -8761,7 +8761,7 @@
       </c>
       <c r="N171">
         <f t="shared" si="11"/>
-        <v>5.3504999999999997E-2</v>
+        <v>4.5157408200000001E-3</v>
       </c>
     </row>
     <row r="172" spans="1:14" x14ac:dyDescent="0.35">
@@ -8803,7 +8803,7 @@
       </c>
       <c r="N172">
         <f t="shared" si="11"/>
-        <v>5.3022999999999994E-2</v>
+        <v>4.5214362299999993E-3</v>
       </c>
     </row>
     <row r="173" spans="1:14" x14ac:dyDescent="0.35">
@@ -8845,7 +8845,7 @@
       </c>
       <c r="N173">
         <f t="shared" si="11"/>
-        <v>5.3440999999999995E-2</v>
+        <v>4.5157969399999996E-3</v>
       </c>
     </row>
     <row r="174" spans="1:14" x14ac:dyDescent="0.35">
@@ -8887,7 +8887,7 @@
       </c>
       <c r="N174">
         <f t="shared" si="11"/>
-        <v>5.6367E-2</v>
+        <v>4.5139705700000003E-3</v>
       </c>
     </row>
     <row r="175" spans="1:14" x14ac:dyDescent="0.35">
@@ -8929,7 +8929,7 @@
       </c>
       <c r="N175">
         <f t="shared" si="11"/>
-        <v>5.6242999999999987E-2</v>
+        <v>4.5141459699999985E-3</v>
       </c>
     </row>
     <row r="176" spans="1:14" x14ac:dyDescent="0.35">
@@ -8971,7 +8971,7 @@
       </c>
       <c r="N176">
         <f t="shared" si="11"/>
-        <v>5.7340000000000002E-2</v>
+        <v>4.5117340199999998E-3</v>
       </c>
     </row>
     <row r="177" spans="1:14" x14ac:dyDescent="0.35">
@@ -9013,7 +9013,7 @@
       </c>
       <c r="N177">
         <f t="shared" si="11"/>
-        <v>5.4505999999999999E-2</v>
+        <v>4.5181858000000004E-3</v>
       </c>
     </row>
     <row r="178" spans="1:14" x14ac:dyDescent="0.35">
@@ -9055,7 +9055,7 @@
       </c>
       <c r="N178">
         <f t="shared" si="11"/>
-        <v>5.7148999999999998E-2</v>
+        <v>4.5119181700000004E-3</v>
       </c>
     </row>
     <row r="179" spans="1:14" x14ac:dyDescent="0.35">
@@ -9097,7 +9097,7 @@
       </c>
       <c r="N179">
         <f t="shared" si="11"/>
-        <v>5.239499999999999E-2</v>
+        <v>4.5274929999999996E-3</v>
       </c>
     </row>
     <row r="180" spans="1:14" x14ac:dyDescent="0.35">
@@ -9139,7 +9139,7 @@
       </c>
       <c r="N180">
         <f t="shared" si="11"/>
-        <v>5.1622000000000001E-2</v>
+        <v>4.5196086700000004E-3</v>
       </c>
     </row>
     <row r="181" spans="1:14" x14ac:dyDescent="0.35">
@@ -9181,7 +9181,7 @@
       </c>
       <c r="N181">
         <f t="shared" si="11"/>
-        <v>5.5892999999999991E-2</v>
+        <v>4.5150195499999999E-3</v>
       </c>
     </row>
     <row r="182" spans="1:14" x14ac:dyDescent="0.35">
@@ -9223,7 +9223,7 @@
       </c>
       <c r="N182">
         <f t="shared" si="11"/>
-        <v>5.5099999999999989E-2</v>
+        <v>4.5168982599999999E-3</v>
       </c>
     </row>
     <row r="183" spans="1:14" x14ac:dyDescent="0.35">
@@ -9265,7 +9265,7 @@
       </c>
       <c r="N183">
         <f t="shared" si="11"/>
-        <v>5.5973000000000002E-2</v>
+        <v>4.5194554799999993E-3</v>
       </c>
     </row>
     <row r="184" spans="1:14" x14ac:dyDescent="0.35">
@@ -9307,7 +9307,7 @@
       </c>
       <c r="N184">
         <f t="shared" si="11"/>
-        <v>5.3032999999999997E-2</v>
+        <v>4.5215941299999998E-3</v>
       </c>
     </row>
     <row r="185" spans="1:14" x14ac:dyDescent="0.35">
@@ -9349,7 +9349,7 @@
       </c>
       <c r="N185">
         <f t="shared" si="11"/>
-        <v>5.5133999999999996E-2</v>
+        <v>4.51212903E-3</v>
       </c>
     </row>
     <row r="186" spans="1:14" x14ac:dyDescent="0.35">
@@ -9391,7 +9391,7 @@
       </c>
       <c r="N186">
         <f t="shared" si="11"/>
-        <v>5.4087000000000003E-2</v>
+        <v>4.523809299999999E-3</v>
       </c>
     </row>
     <row r="187" spans="1:14" x14ac:dyDescent="0.35">
@@ -9433,7 +9433,7 @@
       </c>
       <c r="N187">
         <f t="shared" si="11"/>
-        <v>5.425E-2</v>
+        <v>4.5189436200000002E-3</v>
       </c>
     </row>
     <row r="188" spans="1:14" x14ac:dyDescent="0.35">
@@ -9475,7 +9475,7 @@
       </c>
       <c r="N188">
         <f t="shared" si="11"/>
-        <v>5.3557E-2</v>
+        <v>4.5250407199999999E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>